<commit_message>
updated script by alec
</commit_message>
<xml_diff>
--- a/Cucumber/src/SeleniumExcel.xlsx
+++ b/Cucumber/src/SeleniumExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\git\Test2Shubham\Test1\Cucumber\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\git2\Test1\Cucumber\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6C50B6-4097-4EB4-9101-A484FB420336}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5ACA51-D851-4F1B-BF05-3766A9142F5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37DC1FCF-43AD-40A4-87E8-3E4EA11A1777}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Customer</t>
   </si>
@@ -57,22 +57,16 @@
     <t>shubham</t>
   </si>
   <si>
-    <t>mahendra</t>
-  </si>
-  <si>
-    <t>activa</t>
-  </si>
-  <si>
-    <t>yogendra</t>
-  </si>
-  <si>
-    <t>scooty</t>
-  </si>
-  <si>
-    <t>rahul</t>
-  </si>
-  <si>
-    <t>bullet</t>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Cycle</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>Tractor</t>
   </si>
 </sst>
 </file>
@@ -424,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF2071B-D2B5-428C-A556-0CE07AC6C31B}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,14 +482,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>